<commit_message>
Finish Embedded Software v1.0
</commit_message>
<xml_diff>
--- a/DataFormat/CtrlFormat.xlsx
+++ b/DataFormat/CtrlFormat.xlsx
@@ -8,15 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git_repository\OurEDA\OurEDA-B2S\DataFormat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78334FF1-B959-4994-845A-8F7207D6DA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF720C9-3890-4B97-9333-385ACC907871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>起始位</t>
   </si>
@@ -46,21 +53,6 @@
   </si>
   <si>
     <t>传送</t>
-  </si>
-  <si>
-    <t>机械臂1</t>
-  </si>
-  <si>
-    <t>机械臂2</t>
-  </si>
-  <si>
-    <t>机械臂3</t>
-  </si>
-  <si>
-    <t>机械臂4</t>
-  </si>
-  <si>
-    <t>机械臂5</t>
   </si>
   <si>
     <t>机械臂6</t>
@@ -145,6 +137,29 @@
   <si>
     <t>共30字节</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中臂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小臂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>夹手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大臂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水平</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25 04 D0 05 DC 05 DC 05 DC 05 DC 05 DC 05 DC 05 DC 05 DC 05 DC 05 DC 05 DC 05 DC 08 00 21</t>
   </si>
 </sst>
 </file>
@@ -246,14 +261,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -570,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -583,130 +598,130 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12" t="s">
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12" t="s">
+      <c r="AC1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12" t="s">
+      <c r="AD1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="AE1" s="3"/>
       <c r="AF1" s="4"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA2" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="14"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="AE2" s="7"/>
       <c r="AF2" s="8"/>
@@ -806,107 +821,110 @@
       <c r="AF3" s="8"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="AA5" s="15"/>
+      <c r="AA5" s="13"/>
       <c r="AB5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD5" s="15"/>
+        <v>15</v>
+      </c>
+      <c r="AD5" s="13"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="12"/>
+      <c r="B6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="14"/>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB6" t="s">
         <v>16</v>
       </c>
-      <c r="AB6" t="s">
-        <v>21</v>
-      </c>
       <c r="AC6" s="9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="13"/>
+      <c r="B7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="15"/>
       <c r="F7" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="AB7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="AC7" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AB8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AC8" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="14"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="12"/>
       <c r="AB9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="AC9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD9" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="AD9" s="12"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>39</v>
+      </c>
       <c r="AB12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AB13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -916,6 +934,15 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="V1:W1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="B2:C2"/>
@@ -932,15 +959,6 @@
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>